<commit_message>
Organized some measures, Added more info to the read me file, and grouped some visuals.
</commit_message>
<xml_diff>
--- a/Data/Runs.xlsx
+++ b/Data/Runs.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amwinsusa-my.sharepoint.com/personal/adam_campbell_amwins_com/Documents/Power Bi/Adam Running Report/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amwinsusa-my.sharepoint.com/personal/adam_campbell_amwins_com/Documents/Power Bi/Adam-Running-Report-Power-BI/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2270" documentId="8_{1B5B9EE7-4A87-4B08-8F07-135300A8F237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{044DAF9D-EF75-436B-AA98-2CEF9338BECF}"/>
+  <xr:revisionPtr revIDLastSave="2363" documentId="8_{1B5B9EE7-4A87-4B08-8F07-135300A8F237}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{41C7FEA4-1C95-4DED-9973-07FE531737ED}"/>
   <bookViews>
-    <workbookView xWindow="6600" yWindow="1980" windowWidth="43200" windowHeight="11505" activeTab="3" xr2:uid="{9A847115-9D00-4FBA-8564-3F0597E8F385}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17790" activeTab="1" xr2:uid="{9A847115-9D00-4FBA-8564-3F0597E8F385}"/>
   </bookViews>
   <sheets>
     <sheet name="Runs" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="77">
   <si>
     <t>Date</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>April 20 Runs</t>
+  </si>
+  <si>
+    <t>Littleton</t>
   </si>
 </sst>
 </file>
@@ -656,10 +659,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7F513F-435D-4F41-AA7D-F2F145A3BE11}">
-  <dimension ref="A1:U42"/>
+  <dimension ref="A1:U44"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3284,6 +3288,130 @@
         <v>54</v>
       </c>
     </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A43" s="7">
+        <v>42</v>
+      </c>
+      <c r="B43" s="8">
+        <v>45018</v>
+      </c>
+      <c r="C43" s="9">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="11">
+        <v>4.8</v>
+      </c>
+      <c r="F43" s="11">
+        <v>60.35</v>
+      </c>
+      <c r="G43" s="11">
+        <v>12.26</v>
+      </c>
+      <c r="H43" s="11">
+        <v>9.31</v>
+      </c>
+      <c r="I43" s="7">
+        <v>645</v>
+      </c>
+      <c r="J43" s="7">
+        <v>338</v>
+      </c>
+      <c r="L43" s="7">
+        <v>5618</v>
+      </c>
+      <c r="M43" s="7">
+        <v>163</v>
+      </c>
+      <c r="N43" s="7">
+        <v>181</v>
+      </c>
+      <c r="O43" s="7">
+        <v>137</v>
+      </c>
+      <c r="P43" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q43" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R43" s="7">
+        <v>61</v>
+      </c>
+      <c r="S43" s="7">
+        <v>39</v>
+      </c>
+      <c r="T43" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="U43" s="10" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A44" s="7">
+        <v>43</v>
+      </c>
+      <c r="B44" s="8">
+        <v>45019</v>
+      </c>
+      <c r="C44" s="9">
+        <v>0.40416666666666662</v>
+      </c>
+      <c r="D44" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E44" s="11">
+        <v>4.01</v>
+      </c>
+      <c r="F44" s="11">
+        <v>45.46</v>
+      </c>
+      <c r="G44" s="11">
+        <v>11.25</v>
+      </c>
+      <c r="H44" s="11">
+        <v>11.25</v>
+      </c>
+      <c r="I44" s="7">
+        <v>587</v>
+      </c>
+      <c r="J44" s="7">
+        <v>13</v>
+      </c>
+      <c r="L44" s="7">
+        <v>5528</v>
+      </c>
+      <c r="M44" s="7">
+        <v>160</v>
+      </c>
+      <c r="N44" s="7">
+        <v>181</v>
+      </c>
+      <c r="O44" s="7">
+        <v>146</v>
+      </c>
+      <c r="P44" s="7">
+        <v>1</v>
+      </c>
+      <c r="Q44" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="R44" s="7">
+        <v>41</v>
+      </c>
+      <c r="S44" s="7">
+        <v>39</v>
+      </c>
+      <c r="T44" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="U44" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3292,10 +3420,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7ECB71D-B7B7-4BF4-BA51-D26D84349137}">
-  <dimension ref="A1:F190"/>
+  <dimension ref="A1:F200"/>
   <sheetViews>
-    <sheetView topLeftCell="A157" workbookViewId="0">
-      <selection activeCell="L180" sqref="L180"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J193" sqref="J193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6927,6 +7056,176 @@
       </c>
       <c r="F190" s="7">
         <v>183</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A191" s="7">
+        <v>42</v>
+      </c>
+      <c r="B191" s="7">
+        <v>1</v>
+      </c>
+      <c r="C191" s="11">
+        <v>1</v>
+      </c>
+      <c r="D191" s="11">
+        <v>10.33</v>
+      </c>
+      <c r="F191" s="7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="192" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A192" s="7">
+        <v>42</v>
+      </c>
+      <c r="B192" s="7">
+        <v>2</v>
+      </c>
+      <c r="C192" s="11">
+        <v>1</v>
+      </c>
+      <c r="D192" s="11">
+        <v>13.18</v>
+      </c>
+      <c r="F192" s="7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A193" s="7">
+        <v>42</v>
+      </c>
+      <c r="B193" s="7">
+        <v>3</v>
+      </c>
+      <c r="C193" s="11">
+        <v>1</v>
+      </c>
+      <c r="D193" s="11">
+        <v>13.19</v>
+      </c>
+      <c r="F193" s="7">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="194" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A194" s="7">
+        <v>42</v>
+      </c>
+      <c r="B194" s="7">
+        <v>4</v>
+      </c>
+      <c r="C194" s="11">
+        <v>1</v>
+      </c>
+      <c r="D194" s="11">
+        <v>12.18</v>
+      </c>
+      <c r="F194" s="7">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="195" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A195" s="7">
+        <v>42</v>
+      </c>
+      <c r="B195" s="7">
+        <v>5</v>
+      </c>
+      <c r="C195" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="D195" s="11">
+        <v>13.43</v>
+      </c>
+      <c r="F195" s="7">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A196" s="7">
+        <v>43</v>
+      </c>
+      <c r="B196" s="7">
+        <v>1</v>
+      </c>
+      <c r="C196" s="11">
+        <v>1</v>
+      </c>
+      <c r="D196" s="11">
+        <v>10.47</v>
+      </c>
+      <c r="F196" s="7">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A197" s="7">
+        <v>43</v>
+      </c>
+      <c r="B197" s="7">
+        <v>2</v>
+      </c>
+      <c r="C197" s="11">
+        <v>1</v>
+      </c>
+      <c r="D197" s="11">
+        <v>12.19</v>
+      </c>
+      <c r="F197" s="7">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="198" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A198" s="7">
+        <v>43</v>
+      </c>
+      <c r="B198" s="7">
+        <v>3</v>
+      </c>
+      <c r="C198" s="11">
+        <v>1</v>
+      </c>
+      <c r="D198" s="11">
+        <v>11.13</v>
+      </c>
+      <c r="F198" s="7">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="199" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A199" s="7">
+        <v>43</v>
+      </c>
+      <c r="B199" s="7">
+        <v>4</v>
+      </c>
+      <c r="C199" s="11">
+        <v>1</v>
+      </c>
+      <c r="D199" s="11">
+        <v>11.18</v>
+      </c>
+      <c r="F199" s="7">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="200" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A200" s="7">
+        <v>43</v>
+      </c>
+      <c r="B200" s="7">
+        <v>5</v>
+      </c>
+      <c r="C200" s="11">
+        <v>0.01</v>
+      </c>
+      <c r="D200" s="11">
+        <v>9.44</v>
+      </c>
+      <c r="F200" s="7">
+        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -6997,7 +7296,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{443E1EEC-5E51-4456-ABD4-8D1E13D8D056}">
   <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q17" sqref="Q17"/>
     </sheetView>
   </sheetViews>

</xml_diff>